<commit_message>
Inserir novos itens no Kanban
</commit_message>
<xml_diff>
--- a/projeto/Kanban e PB.xlsx
+++ b/projeto/Kanban e PB.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Projeto Integrador</t>
   </si>
@@ -41,9 +43,6 @@
     <t>Coluna4</t>
   </si>
   <si>
-    <t>Coluna5</t>
-  </si>
-  <si>
     <t>Pesquisa sobre uso de aplicativos para abastecer</t>
   </si>
   <si>
@@ -101,9 +100,6 @@
     <t>Feito</t>
   </si>
   <si>
-    <t xml:space="preserve">Coleta de dados </t>
-  </si>
-  <si>
     <t>Definição das perguntas</t>
   </si>
   <si>
@@ -111,6 +107,15 @@
   </si>
   <si>
     <t>Interface final</t>
+  </si>
+  <si>
+    <t>Montagem de filtros na base de dados</t>
+  </si>
+  <si>
+    <t>Coleta para a base de dados</t>
+  </si>
+  <si>
+    <t>DashBoard</t>
   </si>
 </sst>
 </file>
@@ -197,21 +202,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B5:E10" totalsRowShown="0">
-  <autoFilter ref="B5:E10"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B5:D10" totalsRowShown="0">
+  <autoFilter ref="B5:D10"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Product Backlog"/>
     <tableColumn id="3" name="Sprint Backlog"/>
     <tableColumn id="4" name="Coluna4"/>
-    <tableColumn id="5" name="Coluna5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="B25:D30" totalsRowShown="0">
-  <autoFilter ref="B25:D30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela134" displayName="Tabela134" ref="B3:D8" totalsRowShown="0">
+  <autoFilter ref="B3:D8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="A Fazer"/>
     <tableColumn id="3" name="Fazendo"/>
@@ -520,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="E3:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -582,7 +586,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -596,53 +600,56 @@
       <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -654,141 +661,233 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="2" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="1"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="E30" s="3"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
       <c r="F31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="38.125" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="4" max="4" width="28.875" customWidth="1"/>
+    <col min="5" max="5" width="3.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>

</xml_diff>